<commit_message>
Criacao da pasta e das classes DTO
</commit_message>
<xml_diff>
--- a/esquemaTabelaModelo.xlsx
+++ b/esquemaTabelaModelo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30d42c514d1a9d26/Documentos/GitHub/trabalhoAPIGrupo2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30d42c514d1a9d26/Documentos/GitHub/trabalhoAPIGrupo2/Grupo2-Api-Serratec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{935D75D5-C788-45A3-B423-5E96F0E6C831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69D706FB-A0A2-47B6-AED0-EA9213510670}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="8_{935D75D5-C788-45A3-B423-5E96F0E6C831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64CBD633-2549-4816-8245-C680B01ABA2C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{27354D7C-26F5-4787-9EC6-D7821DA62957}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{27354D7C-26F5-4787-9EC6-D7821DA62957}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -239,6 +239,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -616,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F0543E-4303-4238-A166-671EAA8671CD}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,7 +668,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G1" sqref="G1:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,7 +803,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D1" sqref="D1:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,7 +834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341F4AE2-6511-46AC-BD69-6FC8A8D3D0EE}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
CLasses corpo tudo que pode ser feito sem dto
</commit_message>
<xml_diff>
--- a/esquemaTabelaModelo.xlsx
+++ b/esquemaTabelaModelo.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30d42c514d1a9d26/Documentos/GitHub/trabalhoAPIGrupo2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\api\Grupo2-Api-Serratec\loja_gp2\Grupo2-Api-Serratec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{935D75D5-C788-45A3-B423-5E96F0E6C831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{27354D7C-26F5-4787-9EC6-D7821DA62957}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <sheet name="Categoria" sheetId="6" r:id="rId6"/>
     <sheet name="Log" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>usuário</t>
   </si>
@@ -154,11 +153,23 @@
   <si>
     <t>pedido(List&lt;itens&gt;)</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>priv</t>
+  </si>
+  <si>
+    <t>perfil</t>
+  </si>
+  <si>
+    <t>enun</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -209,10 +220,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60% - Ênfase5" xfId="1" builtinId="48"/>
@@ -528,7 +540,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7DC0A3C-20DF-4149-8586-6B08C034E6E9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -604,11 +616,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F0543E-4303-4238-A166-671EAA8671CD}">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,7 +629,7 @@
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -636,8 +648,21 @@
       <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -646,16 +671,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DFB8893-BED4-48EC-B9EF-B323049CEFD3}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -673,6 +698,9 @@
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -681,11 +709,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B09ED64E-06D6-4CF8-9CBC-FB7385226B6F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,8 +724,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>14</v>
+      <c r="A1" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>20</v>
@@ -724,7 +752,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0441F013-6CB0-4CFF-BE2D-46789D7D582C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -769,16 +797,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B5426B-73FA-4F73-AFB0-B1ACCD539346}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -787,6 +815,9 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -795,7 +826,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341F4AE2-6511-46AC-BD69-6FC8A8D3D0EE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>